<commit_message>
Added: Payment & Post model
</commit_message>
<xml_diff>
--- a/ERD.xlsx
+++ b/ERD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msrez\Documents\STS Workspace\dev-academy-backend-spring-boot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799B9C56-19D1-401D-AF98-33DC8F259D62}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0907D1B0-FC9B-40C5-AFC4-80515F9996DB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{5E8D8D29-071A-41AE-BDC4-2249F0DFE3FA}"/>
   </bookViews>
@@ -223,21 +223,21 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -555,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F272A48C-BFF3-41B0-B4E8-F550D5C4B86F}">
   <dimension ref="B3:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,455 +571,455 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="I3" s="1" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="I3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>101</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="5" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>10001</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="6" t="s">
+      <c r="K5" s="1"/>
+      <c r="L5" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>102</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="5" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="E12" s="3" t="s">
+      <c r="C12" s="5"/>
+      <c r="E12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="H12" s="1" t="s">
+      <c r="F12" s="7"/>
+      <c r="H12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>101</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>1</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>2</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>102</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>2</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="G33" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Added: Create post API
</commit_message>
<xml_diff>
--- a/ERD.xlsx
+++ b/ERD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msrez\Documents\STS Workspace\dev-academy-backend-spring-boot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0907D1B0-FC9B-40C5-AFC4-80515F9996DB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA759F96-9EB2-4CDE-BC3C-45BEABF28B51}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{5E8D8D29-071A-41AE-BDC4-2249F0DFE3FA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>users</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>class_link</t>
+  </si>
+  <si>
+    <t>Introduction Class</t>
+  </si>
+  <si>
+    <t>Sample description</t>
+  </si>
+  <si>
+    <t>www.google.com</t>
   </si>
 </sst>
 </file>
@@ -555,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F272A48C-BFF3-41B0-B4E8-F550D5C4B86F}">
   <dimension ref="B3:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,12 +919,24 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="1">
+        <v>10001</v>
+      </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
@@ -1034,6 +1055,8 @@
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1" xr:uid="{D22AEB5B-7568-47C4-8300-080BA815DF76}"/>
     <hyperlink ref="F6" r:id="rId2" xr:uid="{94B6D1C7-E605-40A1-92F3-7F36C70A7B09}"/>
+    <hyperlink ref="E34" r:id="rId3" xr:uid="{6D057833-3C09-4E6F-8BBF-0231A6346A63}"/>
+    <hyperlink ref="F34" r:id="rId4" xr:uid="{7BA893F7-3A22-425D-BFE0-97E0A705D137}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated: Migrated to online storage
</commit_message>
<xml_diff>
--- a/ERD.xlsx
+++ b/ERD.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msrez\Documents\STS Workspace\dev-academy-backend-spring-boot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA759F96-9EB2-4CDE-BC3C-45BEABF28B51}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BB92B8-F230-4CE9-82DB-87BE432AE7C0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{5E8D8D29-071A-41AE-BDC4-2249F0DFE3FA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23775" windowHeight="7710" xr2:uid="{5E8D8D29-071A-41AE-BDC4-2249F0DFE3FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>users</t>
   </si>
@@ -141,10 +141,19 @@
     <t>Introduction Class</t>
   </si>
   <si>
-    <t>Sample description</t>
-  </si>
-  <si>
     <t>www.google.com</t>
+  </si>
+  <si>
+    <t>resource</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Sample Description</t>
   </si>
 </sst>
 </file>
@@ -176,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -225,12 +234,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -245,6 +265,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -562,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F272A48C-BFF3-41B0-B4E8-F550D5C4B86F}">
-  <dimension ref="B3:L47"/>
+  <dimension ref="B3:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,13 +600,15 @@
     <col min="3" max="4" width="17.5703125" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" customWidth="1"/>
     <col min="10" max="10" width="16.140625" customWidth="1"/>
-    <col min="12" max="12" width="23.140625" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -594,8 +623,9 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -621,13 +651,16 @@
         <v>16</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>101</v>
       </c>
@@ -648,12 +681,13 @@
       <c r="J5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="3" t="s">
+      <c r="K5" s="3"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>102</v>
       </c>
@@ -670,10 +704,11 @@
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="1"/>
+      <c r="K6" s="3"/>
       <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -682,10 +717,11 @@
       <c r="G7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="1"/>
+      <c r="K7" s="3"/>
       <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -694,10 +730,11 @@
       <c r="G8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="1"/>
+      <c r="K8" s="3"/>
       <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -706,10 +743,11 @@
       <c r="G9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="1"/>
+      <c r="K9" s="3"/>
       <c r="L9" s="1"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="1"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
@@ -723,8 +761,9 @@
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
@@ -746,8 +785,9 @@
       <c r="J13" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K13" s="9"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>1</v>
       </c>
@@ -763,8 +803,9 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>2</v>
       </c>
@@ -780,8 +821,9 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K15" s="9"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
@@ -789,36 +831,41 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="9"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="9"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="9"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>25</v>
       </c>
@@ -828,7 +875,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>26</v>
       </c>
@@ -848,7 +895,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -856,7 +903,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -864,7 +911,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -872,7 +919,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -880,7 +927,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -888,17 +935,18 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>33</v>
       </c>
@@ -909,155 +957,175 @@
         <v>15</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="H33" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G34" s="1">
+      <c r="G34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H34" s="1">
         <v>10001</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B32:G32"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="I3:M3"/>
     <mergeCell ref="B23:G23"/>
     <mergeCell ref="H12:J12"/>
+    <mergeCell ref="B32:H32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1" xr:uid="{D22AEB5B-7568-47C4-8300-080BA815DF76}"/>
     <hyperlink ref="F6" r:id="rId2" xr:uid="{94B6D1C7-E605-40A1-92F3-7F36C70A7B09}"/>
-    <hyperlink ref="E34" r:id="rId3" xr:uid="{6D057833-3C09-4E6F-8BBF-0231A6346A63}"/>
-    <hyperlink ref="F34" r:id="rId4" xr:uid="{7BA893F7-3A22-425D-BFE0-97E0A705D137}"/>
+    <hyperlink ref="F34" r:id="rId3" xr:uid="{7BA893F7-3A22-425D-BFE0-97E0A705D137}"/>
+    <hyperlink ref="G34" r:id="rId4" xr:uid="{ED502842-9ED1-4828-B2FE-66A14DA8D98F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>